<commit_message>
Update greedy day heuristic
</commit_message>
<xml_diff>
--- a/carc/c101.xlsx
+++ b/carc/c101.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jinghongmiao/Code/mvt-code/v2/data/raw/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jinghongmiao/Code/mvt-code/v2/data/raw/c101/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A97F9831-8D15-514A-B3EA-863873BC0847}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1A36A5A-05D5-B344-BA5D-06690483499B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-3500" yWindow="-23160" windowWidth="30240" windowHeight="18880" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -21,13 +21,27 @@
     <sheet name="C_dur" sheetId="6" r:id="rId6"/>
     <sheet name="Time_Window" sheetId="7" r:id="rId7"/>
     <sheet name="Min_Nurse" sheetId="8" r:id="rId8"/>
+    <sheet name="Nurse_Type" sheetId="9" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="22">
   <si>
     <t>Parameter</t>
   </si>
@@ -90,6 +104,9 @@
   </si>
   <si>
     <t>LVN</t>
+  </si>
+  <si>
+    <t>Type</t>
   </si>
 </sst>
 </file>
@@ -456,7 +473,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8428,7 +8445,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AY51"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -17609,7 +17628,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:K51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M15" sqref="M15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -17671,10 +17692,10 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>30</v>
+        <v>570</v>
       </c>
       <c r="I2">
-        <v>270</v>
+        <v>810</v>
       </c>
       <c r="J2">
         <v>0</v>
@@ -17712,10 +17733,10 @@
         <v>0</v>
       </c>
       <c r="J3">
-        <v>30</v>
+        <v>570</v>
       </c>
       <c r="K3">
-        <v>270</v>
+        <v>810</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
@@ -17747,10 +17768,10 @@
         <v>0</v>
       </c>
       <c r="J4">
-        <v>30</v>
+        <v>570</v>
       </c>
       <c r="K4">
-        <v>270</v>
+        <v>810</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
@@ -17764,10 +17785,10 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <v>30</v>
+        <v>570</v>
       </c>
       <c r="E5">
-        <v>270</v>
+        <v>810</v>
       </c>
       <c r="F5">
         <v>0</v>
@@ -17805,10 +17826,10 @@
         <v>0</v>
       </c>
       <c r="F6">
-        <v>30</v>
+        <v>570</v>
       </c>
       <c r="G6">
-        <v>270</v>
+        <v>810</v>
       </c>
       <c r="H6">
         <v>0</v>
@@ -17852,10 +17873,10 @@
         <v>0</v>
       </c>
       <c r="J7">
-        <v>30</v>
+        <v>570</v>
       </c>
       <c r="K7">
-        <v>270</v>
+        <v>810</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
@@ -17863,10 +17884,10 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>30</v>
+        <v>570</v>
       </c>
       <c r="C8">
-        <v>270</v>
+        <v>810</v>
       </c>
       <c r="D8">
         <v>0</v>
@@ -17898,10 +17919,10 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>30</v>
+        <v>570</v>
       </c>
       <c r="C9">
-        <v>270</v>
+        <v>810</v>
       </c>
       <c r="D9">
         <v>0</v>
@@ -17933,10 +17954,10 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>30</v>
+        <v>570</v>
       </c>
       <c r="C10">
-        <v>270</v>
+        <v>810</v>
       </c>
       <c r="D10">
         <v>0</v>
@@ -17986,10 +18007,10 @@
         <v>0</v>
       </c>
       <c r="H11">
-        <v>30</v>
+        <v>570</v>
       </c>
       <c r="I11">
-        <v>270</v>
+        <v>810</v>
       </c>
       <c r="J11">
         <v>0</v>
@@ -18027,10 +18048,10 @@
         <v>0</v>
       </c>
       <c r="J12">
-        <v>30</v>
+        <v>570</v>
       </c>
       <c r="K12">
-        <v>270</v>
+        <v>810</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
@@ -18056,10 +18077,10 @@
         <v>0</v>
       </c>
       <c r="H13">
-        <v>30</v>
+        <v>570</v>
       </c>
       <c r="I13">
-        <v>270</v>
+        <v>810</v>
       </c>
       <c r="J13">
         <v>0</v>
@@ -18091,10 +18112,10 @@
         <v>0</v>
       </c>
       <c r="H14">
-        <v>30</v>
+        <v>570</v>
       </c>
       <c r="I14">
-        <v>270</v>
+        <v>810</v>
       </c>
       <c r="J14">
         <v>0</v>
@@ -18114,10 +18135,10 @@
         <v>0</v>
       </c>
       <c r="D15">
-        <v>30</v>
+        <v>570</v>
       </c>
       <c r="E15">
-        <v>270</v>
+        <v>810</v>
       </c>
       <c r="F15">
         <v>0</v>
@@ -18143,10 +18164,10 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <v>30</v>
+        <v>570</v>
       </c>
       <c r="C16">
-        <v>270</v>
+        <v>810</v>
       </c>
       <c r="D16">
         <v>0</v>
@@ -18202,10 +18223,10 @@
         <v>0</v>
       </c>
       <c r="J17">
-        <v>30</v>
+        <v>570</v>
       </c>
       <c r="K17">
-        <v>270</v>
+        <v>810</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
@@ -18231,10 +18252,10 @@
         <v>0</v>
       </c>
       <c r="H18">
-        <v>30</v>
+        <v>570</v>
       </c>
       <c r="I18">
-        <v>270</v>
+        <v>810</v>
       </c>
       <c r="J18">
         <v>0</v>
@@ -18266,10 +18287,10 @@
         <v>0</v>
       </c>
       <c r="H19">
-        <v>30</v>
+        <v>570</v>
       </c>
       <c r="I19">
-        <v>270</v>
+        <v>810</v>
       </c>
       <c r="J19">
         <v>0</v>
@@ -18295,10 +18316,10 @@
         <v>0</v>
       </c>
       <c r="F20">
-        <v>30</v>
+        <v>570</v>
       </c>
       <c r="G20">
-        <v>270</v>
+        <v>810</v>
       </c>
       <c r="H20">
         <v>0</v>
@@ -18330,10 +18351,10 @@
         <v>0</v>
       </c>
       <c r="F21">
-        <v>30</v>
+        <v>570</v>
       </c>
       <c r="G21">
-        <v>270</v>
+        <v>810</v>
       </c>
       <c r="H21">
         <v>0</v>
@@ -18371,10 +18392,10 @@
         <v>0</v>
       </c>
       <c r="H22">
-        <v>30</v>
+        <v>570</v>
       </c>
       <c r="I22">
-        <v>270</v>
+        <v>810</v>
       </c>
       <c r="J22">
         <v>0</v>
@@ -18388,10 +18409,10 @@
         <v>22</v>
       </c>
       <c r="B23">
-        <v>30</v>
+        <v>570</v>
       </c>
       <c r="C23">
-        <v>270</v>
+        <v>810</v>
       </c>
       <c r="D23">
         <v>0</v>
@@ -18441,10 +18462,10 @@
         <v>0</v>
       </c>
       <c r="H24">
-        <v>30</v>
+        <v>570</v>
       </c>
       <c r="I24">
-        <v>270</v>
+        <v>810</v>
       </c>
       <c r="J24">
         <v>0</v>
@@ -18464,10 +18485,10 @@
         <v>0</v>
       </c>
       <c r="D25">
-        <v>30</v>
+        <v>570</v>
       </c>
       <c r="E25">
-        <v>270</v>
+        <v>810</v>
       </c>
       <c r="F25">
         <v>0</v>
@@ -18499,10 +18520,10 @@
         <v>0</v>
       </c>
       <c r="D26">
-        <v>30</v>
+        <v>570</v>
       </c>
       <c r="E26">
-        <v>270</v>
+        <v>810</v>
       </c>
       <c r="F26">
         <v>0</v>
@@ -18552,10 +18573,10 @@
         <v>0</v>
       </c>
       <c r="J27">
-        <v>30</v>
+        <v>570</v>
       </c>
       <c r="K27">
-        <v>270</v>
+        <v>810</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
@@ -18569,10 +18590,10 @@
         <v>0</v>
       </c>
       <c r="D28">
-        <v>30</v>
+        <v>570</v>
       </c>
       <c r="E28">
-        <v>270</v>
+        <v>810</v>
       </c>
       <c r="F28">
         <v>0</v>
@@ -18622,10 +18643,10 @@
         <v>0</v>
       </c>
       <c r="J29">
-        <v>30</v>
+        <v>570</v>
       </c>
       <c r="K29">
-        <v>270</v>
+        <v>810</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.2">
@@ -18639,10 +18660,10 @@
         <v>0</v>
       </c>
       <c r="D30">
-        <v>30</v>
+        <v>570</v>
       </c>
       <c r="E30">
-        <v>270</v>
+        <v>810</v>
       </c>
       <c r="F30">
         <v>0</v>
@@ -18680,10 +18701,10 @@
         <v>0</v>
       </c>
       <c r="F31">
-        <v>30</v>
+        <v>570</v>
       </c>
       <c r="G31">
-        <v>270</v>
+        <v>810</v>
       </c>
       <c r="H31">
         <v>0</v>
@@ -18727,10 +18748,10 @@
         <v>0</v>
       </c>
       <c r="J32">
-        <v>30</v>
+        <v>570</v>
       </c>
       <c r="K32">
-        <v>270</v>
+        <v>810</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.2">
@@ -18738,10 +18759,10 @@
         <v>32</v>
       </c>
       <c r="B33">
-        <v>30</v>
+        <v>570</v>
       </c>
       <c r="C33">
-        <v>270</v>
+        <v>810</v>
       </c>
       <c r="D33">
         <v>0</v>
@@ -18773,10 +18794,10 @@
         <v>33</v>
       </c>
       <c r="B34">
-        <v>30</v>
+        <v>570</v>
       </c>
       <c r="C34">
-        <v>270</v>
+        <v>810</v>
       </c>
       <c r="D34">
         <v>0</v>
@@ -18832,10 +18853,10 @@
         <v>0</v>
       </c>
       <c r="J35">
-        <v>30</v>
+        <v>570</v>
       </c>
       <c r="K35">
-        <v>270</v>
+        <v>810</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.2">
@@ -18843,10 +18864,10 @@
         <v>35</v>
       </c>
       <c r="B36">
-        <v>30</v>
+        <v>570</v>
       </c>
       <c r="C36">
-        <v>270</v>
+        <v>810</v>
       </c>
       <c r="D36">
         <v>0</v>
@@ -18902,10 +18923,10 @@
         <v>0</v>
       </c>
       <c r="J37">
-        <v>30</v>
+        <v>570</v>
       </c>
       <c r="K37">
-        <v>270</v>
+        <v>810</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.2">
@@ -18937,10 +18958,10 @@
         <v>0</v>
       </c>
       <c r="J38">
-        <v>30</v>
+        <v>570</v>
       </c>
       <c r="K38">
-        <v>270</v>
+        <v>810</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.2">
@@ -18966,10 +18987,10 @@
         <v>0</v>
       </c>
       <c r="H39">
-        <v>30</v>
+        <v>570</v>
       </c>
       <c r="I39">
-        <v>270</v>
+        <v>810</v>
       </c>
       <c r="J39">
         <v>0</v>
@@ -19001,10 +19022,10 @@
         <v>0</v>
       </c>
       <c r="H40">
-        <v>30</v>
+        <v>570</v>
       </c>
       <c r="I40">
-        <v>270</v>
+        <v>810</v>
       </c>
       <c r="J40">
         <v>0</v>
@@ -19042,10 +19063,10 @@
         <v>0</v>
       </c>
       <c r="J41">
-        <v>30</v>
+        <v>570</v>
       </c>
       <c r="K41">
-        <v>270</v>
+        <v>810</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.2">
@@ -19071,10 +19092,10 @@
         <v>0</v>
       </c>
       <c r="H42">
-        <v>30</v>
+        <v>570</v>
       </c>
       <c r="I42">
-        <v>270</v>
+        <v>810</v>
       </c>
       <c r="J42">
         <v>0</v>
@@ -19100,10 +19121,10 @@
         <v>0</v>
       </c>
       <c r="F43">
-        <v>30</v>
+        <v>570</v>
       </c>
       <c r="G43">
-        <v>270</v>
+        <v>810</v>
       </c>
       <c r="H43">
         <v>0</v>
@@ -19123,10 +19144,10 @@
         <v>43</v>
       </c>
       <c r="B44">
-        <v>30</v>
+        <v>570</v>
       </c>
       <c r="C44">
-        <v>270</v>
+        <v>810</v>
       </c>
       <c r="D44">
         <v>0</v>
@@ -19182,10 +19203,10 @@
         <v>0</v>
       </c>
       <c r="J45">
-        <v>30</v>
+        <v>570</v>
       </c>
       <c r="K45">
-        <v>270</v>
+        <v>810</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.2">
@@ -19193,10 +19214,10 @@
         <v>45</v>
       </c>
       <c r="B46">
-        <v>30</v>
+        <v>570</v>
       </c>
       <c r="C46">
-        <v>270</v>
+        <v>810</v>
       </c>
       <c r="D46">
         <v>0</v>
@@ -19234,10 +19255,10 @@
         <v>0</v>
       </c>
       <c r="D47">
-        <v>30</v>
+        <v>570</v>
       </c>
       <c r="E47">
-        <v>270</v>
+        <v>810</v>
       </c>
       <c r="F47">
         <v>0</v>
@@ -19263,10 +19284,10 @@
         <v>47</v>
       </c>
       <c r="B48">
-        <v>30</v>
+        <v>570</v>
       </c>
       <c r="C48">
-        <v>270</v>
+        <v>810</v>
       </c>
       <c r="D48">
         <v>0</v>
@@ -19298,10 +19319,10 @@
         <v>48</v>
       </c>
       <c r="B49">
-        <v>30</v>
+        <v>570</v>
       </c>
       <c r="C49">
-        <v>270</v>
+        <v>810</v>
       </c>
       <c r="D49">
         <v>0</v>
@@ -19351,10 +19372,10 @@
         <v>0</v>
       </c>
       <c r="H50">
-        <v>30</v>
+        <v>570</v>
       </c>
       <c r="I50">
-        <v>270</v>
+        <v>810</v>
       </c>
       <c r="J50">
         <v>0</v>
@@ -19386,10 +19407,10 @@
         <v>0</v>
       </c>
       <c r="H51">
-        <v>30</v>
+        <v>570</v>
       </c>
       <c r="I51">
-        <v>270</v>
+        <v>810</v>
       </c>
       <c r="J51">
         <v>0</v>
@@ -19975,4 +19996,427 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{187BD0CE-4648-3A47-94F5-7184764274A6}">
+  <dimension ref="A1:B51"/>
+  <sheetViews>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="J28" sqref="J28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <v>15</v>
+      </c>
+      <c r="B7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
+        <v>17</v>
+      </c>
+      <c r="B8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
+        <v>18</v>
+      </c>
+      <c r="B9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
+        <v>21</v>
+      </c>
+      <c r="B10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
+        <v>22</v>
+      </c>
+      <c r="B11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
+        <v>25</v>
+      </c>
+      <c r="B12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="1">
+        <v>28</v>
+      </c>
+      <c r="B13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="1">
+        <v>30</v>
+      </c>
+      <c r="B14" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="1">
+        <v>33</v>
+      </c>
+      <c r="B15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="1">
+        <v>35</v>
+      </c>
+      <c r="B16" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="1">
+        <v>37</v>
+      </c>
+      <c r="B17" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="1">
+        <v>38</v>
+      </c>
+      <c r="B18" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="1">
+        <v>44</v>
+      </c>
+      <c r="B19" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" s="1">
+        <v>47</v>
+      </c>
+      <c r="B20" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" s="1">
+        <v>49</v>
+      </c>
+      <c r="B21" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" s="1">
+        <v>56</v>
+      </c>
+      <c r="B22" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" s="1">
+        <v>58</v>
+      </c>
+      <c r="B23" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" s="1">
+        <v>60</v>
+      </c>
+      <c r="B24" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" s="1">
+        <v>61</v>
+      </c>
+      <c r="B25" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" s="1">
+        <v>62</v>
+      </c>
+      <c r="B26" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" s="1">
+        <v>63</v>
+      </c>
+      <c r="B27" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" s="1">
+        <v>65</v>
+      </c>
+      <c r="B28" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" s="1">
+        <v>66</v>
+      </c>
+      <c r="B29" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" s="1">
+        <v>68</v>
+      </c>
+      <c r="B30" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31" s="1">
+        <v>69</v>
+      </c>
+      <c r="B31" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32" s="1">
+        <v>70</v>
+      </c>
+      <c r="B32" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" s="1">
+        <v>71</v>
+      </c>
+      <c r="B33" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" s="1">
+        <v>73</v>
+      </c>
+      <c r="B34" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" s="1">
+        <v>75</v>
+      </c>
+      <c r="B35" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36" s="1">
+        <v>76</v>
+      </c>
+      <c r="B36" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37" s="1">
+        <v>77</v>
+      </c>
+      <c r="B37" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38" s="1">
+        <v>79</v>
+      </c>
+      <c r="B38" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39" s="1">
+        <v>80</v>
+      </c>
+      <c r="B39" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A40" s="1">
+        <v>81</v>
+      </c>
+      <c r="B40" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A41" s="1">
+        <v>82</v>
+      </c>
+      <c r="B41" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A42" s="1">
+        <v>86</v>
+      </c>
+      <c r="B42" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A43" s="1">
+        <v>90</v>
+      </c>
+      <c r="B43" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A44" s="1">
+        <v>91</v>
+      </c>
+      <c r="B44" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A45" s="1">
+        <v>92</v>
+      </c>
+      <c r="B45" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A46" s="1">
+        <v>93</v>
+      </c>
+      <c r="B46" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A47" s="1">
+        <v>94</v>
+      </c>
+      <c r="B47" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A48" s="1">
+        <v>96</v>
+      </c>
+      <c r="B48" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A49" s="1">
+        <v>97</v>
+      </c>
+      <c r="B49" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A50" s="1">
+        <v>99</v>
+      </c>
+      <c r="B50" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A51" s="1">
+        <v>100</v>
+      </c>
+      <c r="B51" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update scripts for heuristics
</commit_message>
<xml_diff>
--- a/carc/c101.xlsx
+++ b/carc/c101.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jinghongmiao/Code/mvt-code/v2/data/raw/c101/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jinghongmiao/Code/mvt-code/carc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1A36A5A-05D5-B344-BA5D-06690483499B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5B6BDE1-9E7A-674D-B3BD-746EDCCC9BA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-3500" yWindow="-23160" windowWidth="30240" windowHeight="18880" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="32220" yWindow="-640" windowWidth="30240" windowHeight="18880" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>

</xml_diff>